<commit_message>
generación automática de base de entrenamiento
</commit_message>
<xml_diff>
--- a/data/output/pib_dataset.xlsx
+++ b/data/output/pib_dataset.xlsx
@@ -16,22 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>consumo_privado</t>
+    <t>exportacion_bienes_servicios</t>
   </si>
   <si>
-    <t>inversiones</t>
+    <t>formacion_bruta_capital_fijo</t>
   </si>
   <si>
-    <t>gasto_publico</t>
+    <t>gasto_consumo_final_gobierno_central</t>
   </si>
   <si>
-    <t>exportaciones</t>
+    <t>gasto_consumo_final_hogar_isflsh</t>
   </si>
   <si>
-    <t>importaciones</t>
+    <t>importaciones_bienes_servicios</t>
   </si>
   <si>
-    <t>variacion</t>
+    <t>variacion_existencias</t>
   </si>
   <si>
     <t>pib</t>
@@ -438,7 +438,7 @@
         <v>39994</v>
       </c>
       <c r="B2">
-        <v>7645.8</v>
+        <v>17180.5</v>
       </c>
       <c r="C2">
         <v>12386.8</v>
@@ -447,7 +447,7 @@
         <v>66165.10000000001</v>
       </c>
       <c r="E2">
-        <v>17180.5</v>
+        <v>7645.8</v>
       </c>
       <c r="F2">
         <v>22876</v>
@@ -464,7 +464,7 @@
         <v>40086</v>
       </c>
       <c r="B3">
-        <v>8728.9</v>
+        <v>16196.5</v>
       </c>
       <c r="C3">
         <v>11359.1</v>
@@ -473,7 +473,7 @@
         <v>65711.89999999999</v>
       </c>
       <c r="E3">
-        <v>16196.5</v>
+        <v>8728.9</v>
       </c>
       <c r="F3">
         <v>25296.9</v>
@@ -490,7 +490,7 @@
         <v>40178</v>
       </c>
       <c r="B4">
-        <v>9664.6</v>
+        <v>18393.6</v>
       </c>
       <c r="C4">
         <v>12432.4</v>
@@ -499,7 +499,7 @@
         <v>67381.60000000001</v>
       </c>
       <c r="E4">
-        <v>18393.6</v>
+        <v>9664.6</v>
       </c>
       <c r="F4">
         <v>27584.6</v>
@@ -516,7 +516,7 @@
         <v>40268</v>
       </c>
       <c r="B5">
-        <v>7904.4</v>
+        <v>20262</v>
       </c>
       <c r="C5">
         <v>12062.5</v>
@@ -525,7 +525,7 @@
         <v>69048.8</v>
       </c>
       <c r="E5">
-        <v>20262</v>
+        <v>7904.4</v>
       </c>
       <c r="F5">
         <v>26222.3</v>
@@ -542,7 +542,7 @@
         <v>40359</v>
       </c>
       <c r="B6">
-        <v>8587.799999999999</v>
+        <v>20276.9</v>
       </c>
       <c r="C6">
         <v>12647</v>
@@ -551,7 +551,7 @@
         <v>70970</v>
       </c>
       <c r="E6">
-        <v>20276.9</v>
+        <v>8587.799999999999</v>
       </c>
       <c r="F6">
         <v>28017</v>
@@ -568,7 +568,7 @@
         <v>40451</v>
       </c>
       <c r="B7">
-        <v>9372.299999999999</v>
+        <v>18265.9</v>
       </c>
       <c r="C7">
         <v>12992.1</v>
@@ -577,7 +577,7 @@
         <v>71505.5</v>
       </c>
       <c r="E7">
-        <v>18265.9</v>
+        <v>9372.299999999999</v>
       </c>
       <c r="F7">
         <v>29916.7</v>
@@ -594,7 +594,7 @@
         <v>40543</v>
       </c>
       <c r="B8">
-        <v>10905.7</v>
+        <v>20515.3</v>
       </c>
       <c r="C8">
         <v>13799.9</v>
@@ -603,7 +603,7 @@
         <v>74355.2</v>
       </c>
       <c r="E8">
-        <v>20515.3</v>
+        <v>10905.7</v>
       </c>
       <c r="F8">
         <v>31771.3</v>
@@ -620,7 +620,7 @@
         <v>40633</v>
       </c>
       <c r="B9">
-        <v>8665.1</v>
+        <v>23866.7</v>
       </c>
       <c r="C9">
         <v>13626.1</v>
@@ -629,7 +629,7 @@
         <v>76958.7</v>
       </c>
       <c r="E9">
-        <v>23866.7</v>
+        <v>8665.1</v>
       </c>
       <c r="F9">
         <v>32232.3</v>
@@ -646,7 +646,7 @@
         <v>40724</v>
       </c>
       <c r="B10">
-        <v>9508.200000000001</v>
+        <v>22583.7</v>
       </c>
       <c r="C10">
         <v>13823.5</v>
@@ -655,7 +655,7 @@
         <v>76498.5</v>
       </c>
       <c r="E10">
-        <v>22583.7</v>
+        <v>9508.200000000001</v>
       </c>
       <c r="F10">
         <v>33967.6</v>
@@ -672,7 +672,7 @@
         <v>40816</v>
       </c>
       <c r="B11">
-        <v>10040.5</v>
+        <v>22352.8</v>
       </c>
       <c r="C11">
         <v>14684.1</v>
@@ -681,7 +681,7 @@
         <v>80654.7</v>
       </c>
       <c r="E11">
-        <v>22352.8</v>
+        <v>10040.5</v>
       </c>
       <c r="F11">
         <v>35720</v>
@@ -698,7 +698,7 @@
         <v>40908</v>
       </c>
       <c r="B12">
-        <v>11787.5</v>
+        <v>22162</v>
       </c>
       <c r="C12">
         <v>15441</v>
@@ -707,7 +707,7 @@
         <v>81055.10000000001</v>
       </c>
       <c r="E12">
-        <v>22162</v>
+        <v>11787.5</v>
       </c>
       <c r="F12">
         <v>34100.5</v>
@@ -724,7 +724,7 @@
         <v>40999</v>
       </c>
       <c r="B13">
-        <v>9450</v>
+        <v>24171.8</v>
       </c>
       <c r="C13">
         <v>14820.7</v>
@@ -733,7 +733,7 @@
         <v>84395.5</v>
       </c>
       <c r="E13">
-        <v>24171.8</v>
+        <v>9450</v>
       </c>
       <c r="F13">
         <v>35199.1</v>
@@ -750,7 +750,7 @@
         <v>41090</v>
       </c>
       <c r="B14">
-        <v>9657.9</v>
+        <v>22011.5</v>
       </c>
       <c r="C14">
         <v>15216.6</v>
@@ -759,7 +759,7 @@
         <v>81625.5</v>
       </c>
       <c r="E14">
-        <v>22011.5</v>
+        <v>9657.9</v>
       </c>
       <c r="F14">
         <v>34055.8</v>
@@ -776,7 +776,7 @@
         <v>41182</v>
       </c>
       <c r="B15">
-        <v>10915.8</v>
+        <v>21455.4</v>
       </c>
       <c r="C15">
         <v>15110.2</v>
@@ -785,7 +785,7 @@
         <v>83050.8</v>
       </c>
       <c r="E15">
-        <v>21455.4</v>
+        <v>10915.8</v>
       </c>
       <c r="F15">
         <v>34474.9</v>
@@ -802,7 +802,7 @@
         <v>41274</v>
       </c>
       <c r="B16">
-        <v>13415.9</v>
+        <v>21933.5</v>
       </c>
       <c r="C16">
         <v>16414.4</v>
@@ -811,7 +811,7 @@
         <v>86717.39999999999</v>
       </c>
       <c r="E16">
-        <v>21933.5</v>
+        <v>13415.9</v>
       </c>
       <c r="F16">
         <v>36369.7</v>
@@ -828,7 +828,7 @@
         <v>41364</v>
       </c>
       <c r="B17">
-        <v>9430.139999999999</v>
+        <v>23778.57</v>
       </c>
       <c r="C17">
         <v>14521.32</v>
@@ -837,7 +837,7 @@
         <v>85731.61</v>
       </c>
       <c r="E17">
-        <v>23778.57</v>
+        <v>9430.139999999999</v>
       </c>
       <c r="F17">
         <v>34315.33</v>
@@ -854,7 +854,7 @@
         <v>41455</v>
       </c>
       <c r="B18">
-        <v>11800.43</v>
+        <v>23284.22</v>
       </c>
       <c r="C18">
         <v>15653.6</v>
@@ -863,7 +863,7 @@
         <v>88630.94</v>
       </c>
       <c r="E18">
-        <v>23284.22</v>
+        <v>11800.43</v>
       </c>
       <c r="F18">
         <v>36399.45</v>
@@ -880,7 +880,7 @@
         <v>41547</v>
       </c>
       <c r="B19">
-        <v>12004.06</v>
+        <v>21766.35</v>
       </c>
       <c r="C19">
         <v>16060.58</v>
@@ -889,7 +889,7 @@
         <v>89423.33</v>
       </c>
       <c r="E19">
-        <v>21766.35</v>
+        <v>12004.06</v>
       </c>
       <c r="F19">
         <v>36633.45</v>
@@ -906,7 +906,7 @@
         <v>41639</v>
       </c>
       <c r="B20">
-        <v>13766.49</v>
+        <v>22767.49</v>
       </c>
       <c r="C20">
         <v>16599.08</v>
@@ -915,7 +915,7 @@
         <v>92464.67</v>
       </c>
       <c r="E20">
-        <v>22767.49</v>
+        <v>13766.49</v>
       </c>
       <c r="F20">
         <v>37082.89</v>
@@ -932,7 +932,7 @@
         <v>41729</v>
       </c>
       <c r="B21">
-        <v>10326.9</v>
+        <v>24335.8</v>
       </c>
       <c r="C21">
         <v>15781.53</v>
@@ -941,7 +941,7 @@
         <v>91248.72</v>
       </c>
       <c r="E21">
-        <v>24335.8</v>
+        <v>10326.9</v>
       </c>
       <c r="F21">
         <v>35612.86</v>
@@ -958,7 +958,7 @@
         <v>41820</v>
       </c>
       <c r="B22">
-        <v>12334.79</v>
+        <v>24870.08</v>
       </c>
       <c r="C22">
         <v>16955.55</v>
@@ -967,7 +967,7 @@
         <v>94483.36</v>
       </c>
       <c r="E22">
-        <v>24870.08</v>
+        <v>12334.79</v>
       </c>
       <c r="F22">
         <v>37806.95</v>
@@ -984,7 +984,7 @@
         <v>41912</v>
       </c>
       <c r="B23">
-        <v>12904.12</v>
+        <v>24269.49</v>
       </c>
       <c r="C23">
         <v>17134.95</v>
@@ -993,7 +993,7 @@
         <v>96950.88</v>
       </c>
       <c r="E23">
-        <v>24269.49</v>
+        <v>12904.12</v>
       </c>
       <c r="F23">
         <v>38199.08</v>
@@ -1010,7 +1010,7 @@
         <v>42004</v>
       </c>
       <c r="B24">
-        <v>14782.49</v>
+        <v>23792.89</v>
       </c>
       <c r="C24">
         <v>17995.33</v>
@@ -1019,7 +1019,7 @@
         <v>98743.28999999999</v>
       </c>
       <c r="E24">
-        <v>23792.89</v>
+        <v>14782.49</v>
       </c>
       <c r="F24">
         <v>37514.85</v>
@@ -1036,7 +1036,7 @@
         <v>42094</v>
       </c>
       <c r="B25">
-        <v>11855.61</v>
+        <v>24243.48</v>
       </c>
       <c r="C25">
         <v>16063.27</v>
@@ -1045,7 +1045,7 @@
         <v>96635.61</v>
       </c>
       <c r="E25">
-        <v>24243.48</v>
+        <v>11855.61</v>
       </c>
       <c r="F25">
         <v>33930.11</v>
@@ -1062,7 +1062,7 @@
         <v>42185</v>
       </c>
       <c r="B26">
-        <v>12492.36</v>
+        <v>24496.68</v>
       </c>
       <c r="C26">
         <v>16287.52</v>
@@ -1071,7 +1071,7 @@
         <v>98920.10000000001</v>
       </c>
       <c r="E26">
-        <v>24496.68</v>
+        <v>12492.36</v>
       </c>
       <c r="F26">
         <v>35436.5</v>
@@ -1088,7 +1088,7 @@
         <v>42277</v>
       </c>
       <c r="B27">
-        <v>13431.81</v>
+        <v>23367</v>
       </c>
       <c r="C27">
         <v>17793.54</v>
@@ -1097,7 +1097,7 @@
         <v>101467.1</v>
       </c>
       <c r="E27">
-        <v>23367</v>
+        <v>13431.81</v>
       </c>
       <c r="F27">
         <v>37265.87</v>
@@ -1114,7 +1114,7 @@
         <v>42369</v>
       </c>
       <c r="B28">
-        <v>15002.14</v>
+        <v>22287.72</v>
       </c>
       <c r="C28">
         <v>18957.91</v>
@@ -1123,7 +1123,7 @@
         <v>104347.14</v>
       </c>
       <c r="E28">
-        <v>22287.72</v>
+        <v>15002.14</v>
       </c>
       <c r="F28">
         <v>36476.86</v>
@@ -1140,7 +1140,7 @@
         <v>42460</v>
       </c>
       <c r="B29">
-        <v>11252.32</v>
+        <v>23867.37</v>
       </c>
       <c r="C29">
         <v>16061.27</v>
@@ -1149,7 +1149,7 @@
         <v>102827.45</v>
       </c>
       <c r="E29">
-        <v>23867.37</v>
+        <v>11252.32</v>
       </c>
       <c r="F29">
         <v>32290.62</v>
@@ -1166,7 +1166,7 @@
         <v>42551</v>
       </c>
       <c r="B30">
-        <v>11552.85</v>
+        <v>24118.64</v>
       </c>
       <c r="C30">
         <v>17445.98</v>
@@ -1175,7 +1175,7 @@
         <v>105141.61</v>
       </c>
       <c r="E30">
-        <v>24118.64</v>
+        <v>11552.85</v>
       </c>
       <c r="F30">
         <v>35363.92</v>
@@ -1192,7 +1192,7 @@
         <v>42643</v>
       </c>
       <c r="B31">
-        <v>13968.34</v>
+        <v>22703.15</v>
       </c>
       <c r="C31">
         <v>17127.94</v>
@@ -1201,7 +1201,7 @@
         <v>106775.98</v>
       </c>
       <c r="E31">
-        <v>22703.15</v>
+        <v>13968.34</v>
       </c>
       <c r="F31">
         <v>34730.6</v>
@@ -1218,7 +1218,7 @@
         <v>42735</v>
       </c>
       <c r="B32">
-        <v>15637.24</v>
+        <v>23451.67</v>
       </c>
       <c r="C32">
         <v>19001.06</v>
@@ -1227,7 +1227,7 @@
         <v>109768.87</v>
       </c>
       <c r="E32">
-        <v>23451.67</v>
+        <v>15637.24</v>
       </c>
       <c r="F32">
         <v>36265.97</v>
@@ -1244,7 +1244,7 @@
         <v>42825</v>
       </c>
       <c r="B33">
-        <v>11742.32</v>
+        <v>25904.65</v>
       </c>
       <c r="C33">
         <v>16797.89</v>
@@ -1253,7 +1253,7 @@
         <v>108265.29</v>
       </c>
       <c r="E33">
-        <v>25904.65</v>
+        <v>11742.32</v>
       </c>
       <c r="F33">
         <v>34647.15</v>
@@ -1270,7 +1270,7 @@
         <v>42916</v>
       </c>
       <c r="B34">
-        <v>11995.86</v>
+        <v>24993.89</v>
       </c>
       <c r="C34">
         <v>17179.23</v>
@@ -1279,7 +1279,7 @@
         <v>109436.69</v>
       </c>
       <c r="E34">
-        <v>24993.89</v>
+        <v>11995.86</v>
       </c>
       <c r="F34">
         <v>34858.4</v>
@@ -1296,7 +1296,7 @@
         <v>43008</v>
       </c>
       <c r="B35">
-        <v>14345.69</v>
+        <v>23188.11</v>
       </c>
       <c r="C35">
         <v>18703.37</v>
@@ -1305,7 +1305,7 @@
         <v>112095.83</v>
       </c>
       <c r="E35">
-        <v>23188.11</v>
+        <v>14345.69</v>
       </c>
       <c r="F35">
         <v>35960.84</v>
@@ -1322,7 +1322,7 @@
         <v>43100</v>
       </c>
       <c r="B36">
-        <v>17582.83</v>
+        <v>23291.14</v>
       </c>
       <c r="C36">
         <v>18974.17</v>
@@ -1331,7 +1331,7 @@
         <v>117261.74</v>
       </c>
       <c r="E36">
-        <v>23291.14</v>
+        <v>17582.83</v>
       </c>
       <c r="F36">
         <v>39714.73</v>
@@ -1348,7 +1348,7 @@
         <v>43190</v>
       </c>
       <c r="B37">
-        <v>12758.97</v>
+        <v>25389.07</v>
       </c>
       <c r="C37">
         <v>17034</v>
@@ -1357,7 +1357,7 @@
         <v>113161.65</v>
       </c>
       <c r="E37">
-        <v>25389.07</v>
+        <v>12758.97</v>
       </c>
       <c r="F37">
         <v>35608.78</v>
@@ -1374,7 +1374,7 @@
         <v>43281</v>
       </c>
       <c r="B38">
-        <v>13812.74</v>
+        <v>25476.24</v>
       </c>
       <c r="C38">
         <v>18725</v>
@@ -1383,7 +1383,7 @@
         <v>115969.39</v>
       </c>
       <c r="E38">
-        <v>25476.24</v>
+        <v>13812.74</v>
       </c>
       <c r="F38">
         <v>40255.53</v>
@@ -1400,7 +1400,7 @@
         <v>43373</v>
       </c>
       <c r="B39">
-        <v>16109.34</v>
+        <v>24666.81</v>
       </c>
       <c r="C39">
         <v>19486.35</v>
@@ -1409,7 +1409,7 @@
         <v>119179.46</v>
       </c>
       <c r="E39">
-        <v>24666.81</v>
+        <v>16109.34</v>
       </c>
       <c r="F39">
         <v>40584.92</v>
@@ -1426,7 +1426,7 @@
         <v>43465</v>
       </c>
       <c r="B40">
-        <v>18632.5</v>
+        <v>24647.75</v>
       </c>
       <c r="C40">
         <v>20269.45</v>
@@ -1435,7 +1435,7 @@
         <v>124555.71</v>
       </c>
       <c r="E40">
-        <v>24647.75</v>
+        <v>18632.5</v>
       </c>
       <c r="F40">
         <v>42578.31</v>
@@ -1452,7 +1452,7 @@
         <v>43555</v>
       </c>
       <c r="B41">
-        <v>13665.33</v>
+        <v>26350.63</v>
       </c>
       <c r="C41">
         <v>18858.3</v>
@@ -1461,7 +1461,7 @@
         <v>121527.27</v>
       </c>
       <c r="E41">
-        <v>26350.63</v>
+        <v>13665.33</v>
       </c>
       <c r="F41">
         <v>39631.34</v>
@@ -1478,7 +1478,7 @@
         <v>43646</v>
       </c>
       <c r="B42">
-        <v>14609.2</v>
+        <v>26529.72</v>
       </c>
       <c r="C42">
         <v>21780.48</v>
@@ -1487,7 +1487,7 @@
         <v>124206.7</v>
       </c>
       <c r="E42">
-        <v>26529.72</v>
+        <v>14609.2</v>
       </c>
       <c r="F42">
         <v>40851.34</v>
@@ -1504,7 +1504,7 @@
         <v>43738</v>
       </c>
       <c r="B43">
-        <v>17509.59</v>
+        <v>25727.8</v>
       </c>
       <c r="C43">
         <v>21907.27</v>
@@ -1513,7 +1513,7 @@
         <v>126417.03</v>
       </c>
       <c r="E43">
-        <v>25727.8</v>
+        <v>17509.59</v>
       </c>
       <c r="F43">
         <v>41482.82</v>
@@ -1530,7 +1530,7 @@
         <v>43830</v>
       </c>
       <c r="B44">
-        <v>20188.38</v>
+        <v>26002.06</v>
       </c>
       <c r="C44">
         <v>22862.93</v>
@@ -1539,7 +1539,7 @@
         <v>131869.59</v>
       </c>
       <c r="E44">
-        <v>26002.06</v>
+        <v>20188.38</v>
       </c>
       <c r="F44">
         <v>43781.01</v>
@@ -1556,7 +1556,7 @@
         <v>43921</v>
       </c>
       <c r="B45">
-        <v>14332.93</v>
+        <v>27538.38</v>
       </c>
       <c r="C45">
         <v>19336.23</v>
@@ -1565,7 +1565,7 @@
         <v>124497.43</v>
       </c>
       <c r="E45">
-        <v>27538.38</v>
+        <v>14332.93</v>
       </c>
       <c r="F45">
         <v>39435.21</v>
@@ -1582,7 +1582,7 @@
         <v>44012</v>
       </c>
       <c r="B46">
-        <v>14897.08</v>
+        <v>21895.37</v>
       </c>
       <c r="C46">
         <v>18519.86</v>
@@ -1591,7 +1591,7 @@
         <v>113987.8</v>
       </c>
       <c r="E46">
-        <v>21895.37</v>
+        <v>14897.08</v>
       </c>
       <c r="F46">
         <v>31400.47</v>
@@ -1608,7 +1608,7 @@
         <v>44104</v>
       </c>
       <c r="B47">
-        <v>17888.81</v>
+        <v>23306.82</v>
       </c>
       <c r="C47">
         <v>21291.87</v>
@@ -1617,7 +1617,7 @@
         <v>126716.85</v>
       </c>
       <c r="E47">
-        <v>23306.82</v>
+        <v>17888.81</v>
       </c>
       <c r="F47">
         <v>35680.23</v>
@@ -1634,7 +1634,7 @@
         <v>44196</v>
       </c>
       <c r="B48">
-        <v>21727.07</v>
+        <v>25341.13</v>
       </c>
       <c r="C48">
         <v>23083.59</v>
@@ -1643,7 +1643,7 @@
         <v>135785.48</v>
       </c>
       <c r="E48">
-        <v>25341.13</v>
+        <v>21727.07</v>
       </c>
       <c r="F48">
         <v>42297.36</v>
@@ -1660,7 +1660,7 @@
         <v>44286</v>
       </c>
       <c r="B49">
-        <v>15335.99</v>
+        <v>28225.76</v>
       </c>
       <c r="C49">
         <v>24280.23</v>
@@ -1669,7 +1669,7 @@
         <v>137035.27</v>
       </c>
       <c r="E49">
-        <v>28225.76</v>
+        <v>15335.99</v>
       </c>
       <c r="F49">
         <v>45182.97</v>
@@ -1686,7 +1686,7 @@
         <v>44377</v>
       </c>
       <c r="B50">
-        <v>16965.33</v>
+        <v>29053.21</v>
       </c>
       <c r="C50">
         <v>26063.64</v>
@@ -1695,7 +1695,7 @@
         <v>138196.2</v>
       </c>
       <c r="E50">
-        <v>29053.21</v>
+        <v>16965.33</v>
       </c>
       <c r="F50">
         <v>51033.38</v>
@@ -1712,7 +1712,7 @@
         <v>44469</v>
       </c>
       <c r="B51">
-        <v>19303.82</v>
+        <v>30006.58</v>
       </c>
       <c r="C51">
         <v>28472.39</v>
@@ -1721,7 +1721,7 @@
         <v>144978.03</v>
       </c>
       <c r="E51">
-        <v>30006.58</v>
+        <v>19303.82</v>
       </c>
       <c r="F51">
         <v>54700.43</v>
@@ -1738,7 +1738,7 @@
         <v>44561</v>
       </c>
       <c r="B52">
-        <v>23503.51</v>
+        <v>30600.54</v>
       </c>
       <c r="C52">
         <v>29050.01</v>
@@ -1747,7 +1747,7 @@
         <v>154904.38</v>
       </c>
       <c r="E52">
-        <v>30600.54</v>
+        <v>23503.51</v>
       </c>
       <c r="F52">
         <v>60596.87</v>
@@ -1764,7 +1764,7 @@
         <v>44651</v>
       </c>
       <c r="B53">
-        <v>17180.01</v>
+        <v>34901.81</v>
       </c>
       <c r="C53">
         <v>29800.35</v>
@@ -1773,7 +1773,7 @@
         <v>154730.28</v>
       </c>
       <c r="E53">
-        <v>34901.81</v>
+        <v>17180.01</v>
       </c>
       <c r="F53">
         <v>62183.18</v>
@@ -1790,7 +1790,7 @@
         <v>44742</v>
       </c>
       <c r="B54">
-        <v>18950.02</v>
+        <v>36763.29</v>
       </c>
       <c r="C54">
         <v>29923.77</v>
@@ -1799,7 +1799,7 @@
         <v>159866.86</v>
       </c>
       <c r="E54">
-        <v>36763.29</v>
+        <v>18950.02</v>
       </c>
       <c r="F54">
         <v>67025.05</v>
@@ -1816,7 +1816,7 @@
         <v>44834</v>
       </c>
       <c r="B55">
-        <v>21881.11</v>
+        <v>34988.86</v>
       </c>
       <c r="C55">
         <v>31955.14</v>
@@ -1825,7 +1825,7 @@
         <v>166286.69</v>
       </c>
       <c r="E55">
-        <v>34988.86</v>
+        <v>21881.11</v>
       </c>
       <c r="F55">
         <v>68476.07000000001</v>
@@ -1842,7 +1842,7 @@
         <v>44926</v>
       </c>
       <c r="B56">
-        <v>27019.03</v>
+        <v>33742.28</v>
       </c>
       <c r="C56">
         <v>32093.43</v>
@@ -1851,7 +1851,7 @@
         <v>174720.37</v>
       </c>
       <c r="E56">
-        <v>33742.28</v>
+        <v>27019.03</v>
       </c>
       <c r="F56">
         <v>65249.7</v>
@@ -1868,7 +1868,7 @@
         <v>45016</v>
       </c>
       <c r="B57">
-        <v>20622.29</v>
+        <v>36177.39</v>
       </c>
       <c r="C57">
         <v>31896.19</v>
@@ -1877,7 +1877,7 @@
         <v>172616.53</v>
       </c>
       <c r="E57">
-        <v>36177.39</v>
+        <v>20622.29</v>
       </c>
       <c r="F57">
         <v>61820.93</v>
@@ -1894,7 +1894,7 @@
         <v>45107</v>
       </c>
       <c r="B58">
-        <v>23129.23</v>
+        <v>34678.17</v>
       </c>
       <c r="C58">
         <v>31663.98</v>
@@ -1903,7 +1903,7 @@
         <v>175761.43</v>
       </c>
       <c r="E58">
-        <v>34678.17</v>
+        <v>23129.23</v>
       </c>
       <c r="F58">
         <v>64363.65</v>
@@ -1920,7 +1920,7 @@
         <v>45199</v>
       </c>
       <c r="B59">
-        <v>23189.9</v>
+        <v>33039.01</v>
       </c>
       <c r="C59">
         <v>34766.21</v>
@@ -1929,7 +1929,7 @@
         <v>179216.82</v>
       </c>
       <c r="E59">
-        <v>33039.01</v>
+        <v>23189.9</v>
       </c>
       <c r="F59">
         <v>66146.42</v>
@@ -1946,7 +1946,7 @@
         <v>45291</v>
       </c>
       <c r="B60">
-        <v>24929.79</v>
+        <v>31587.4</v>
       </c>
       <c r="C60">
         <v>34067.36</v>
@@ -1955,7 +1955,7 @@
         <v>187342.98</v>
       </c>
       <c r="E60">
-        <v>31587.4</v>
+        <v>24929.79</v>
       </c>
       <c r="F60">
         <v>66394.61</v>
@@ -1972,7 +1972,7 @@
         <v>45382</v>
       </c>
       <c r="B61">
-        <v>20670.85</v>
+        <v>34838.92</v>
       </c>
       <c r="C61">
         <v>32898.42</v>
@@ -1981,7 +1981,7 @@
         <v>186251.67</v>
       </c>
       <c r="E61">
-        <v>34838.92</v>
+        <v>20670.85</v>
       </c>
       <c r="F61">
         <v>66138.42999999999</v>
@@ -1998,7 +1998,7 @@
         <v>45473</v>
       </c>
       <c r="B62">
-        <v>21631.61</v>
+        <v>36378.46</v>
       </c>
       <c r="C62">
         <v>33643.2</v>
@@ -2007,7 +2007,7 @@
         <v>190042.81</v>
       </c>
       <c r="E62">
-        <v>36378.46</v>
+        <v>21631.61</v>
       </c>
       <c r="F62">
         <v>69394.14999999999</v>

</xml_diff>

<commit_message>
modificacion nombres variables target
</commit_message>
<xml_diff>
--- a/data/output/pib_dataset.xlsx
+++ b/data/output/pib_dataset.xlsx
@@ -16,22 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>exportacion_bienes_servicios</t>
+    <t>exportaciones</t>
   </si>
   <si>
-    <t>formacion_bruta_capital_fijo</t>
+    <t>inversiones</t>
   </si>
   <si>
-    <t>gasto_consumo_final_gobierno_central</t>
+    <t>gasto_publico</t>
   </si>
   <si>
-    <t>gasto_consumo_final_hogar_isflsh</t>
+    <t>consumo_privado</t>
   </si>
   <si>
-    <t>importaciones_bienes_servicios</t>
+    <t>importaciones</t>
   </si>
   <si>
-    <t>variacion_existencias</t>
+    <t>variacion</t>
   </si>
   <si>
     <t>pib</t>

</xml_diff>